<commit_message>
NEW: ST7789 LCD 验证成功出图
</commit_message>
<xml_diff>
--- a/F429引脚统计.xlsx
+++ b/F429引脚统计.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB8B46D-2795-40DA-BFC1-4429D6F65703}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E886449C-21B5-4AE6-9A1E-DE5F0A111F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="238">
   <si>
     <t>外设</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -198,10 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SPI3_SDA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PB3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -912,6 +908,22 @@
   </si>
   <si>
     <t>硬件接反了，程序已验证，待改版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI3_SDA(MOSI)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未引出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MISO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -935,7 +947,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,12 +969,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,9 +1023,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1032,17 +1035,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1050,16 +1047,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1342,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1384,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1">
         <v>0</v>
@@ -1396,14 +1402,14 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1419,28 +1425,28 @@
         <v>0</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="11">
-        <v>1</v>
-      </c>
-      <c r="M2" s="11">
+      <c r="K2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1454,24 +1460,24 @@
         <v>0</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="11">
-        <v>1</v>
-      </c>
-      <c r="M3" s="11">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="10">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1485,17 +1491,17 @@
         <v>0</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>104</v>
+      <c r="H4" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L4" s="7">
         <v>1</v>
@@ -1503,13 +1509,13 @@
       <c r="M4" s="7">
         <v>0</v>
       </c>
-      <c r="N4" s="16" t="s">
-        <v>149</v>
+      <c r="N4" s="22" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1523,13 +1529,13 @@
         <v>2</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L5" s="7">
         <v>1</v>
@@ -1537,11 +1543,11 @@
       <c r="M5" s="7">
         <v>0</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1549,23 +1555,23 @@
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -1575,8 +1581,8 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1590,350 +1596,350 @@
         <v>0</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="L8" s="12">
+        <v>1</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="L10" s="12">
+        <v>1</v>
+      </c>
+      <c r="M10" s="12">
         <v>2</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="13" t="s">
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L8" s="13">
-        <v>1</v>
-      </c>
-      <c r="M8" s="13">
-        <v>0</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="13">
-        <v>1</v>
-      </c>
-      <c r="M9" s="13">
-        <v>0</v>
-      </c>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="L10" s="13">
-        <v>1</v>
-      </c>
-      <c r="M10" s="13">
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="11">
+        <v>1</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" s="11">
+        <v>1</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="11">
+        <v>1</v>
+      </c>
+      <c r="M15" s="11">
         <v>2</v>
       </c>
-      <c r="N10" s="21"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="9">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="9">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="L13" s="12">
-        <v>1</v>
-      </c>
-      <c r="M13" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L14" s="12">
-        <v>1</v>
-      </c>
-      <c r="M14" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="L15" s="12">
-        <v>1</v>
-      </c>
-      <c r="M15" s="12">
-        <v>2</v>
-      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="14" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="18" t="s">
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I16" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="M16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="L17" s="4">
         <v>1</v>
@@ -1949,32 +1955,32 @@
       <c r="B18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="15">
         <v>2</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>106</v>
+        <v>151</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="L18" s="1">
         <v>1</v>
@@ -1986,28 +1992,28 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="8">
-        <v>1</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="D19" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15">
         <v>0</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="19"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
@@ -2019,30 +2025,30 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E20" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="15">
         <v>0</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
@@ -2051,798 +2057,793 @@
         <v>3</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="C21" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15">
         <v>0</v>
       </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="8">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="F22" s="15">
         <v>0</v>
       </c>
       <c r="G22" s="17"/>
       <c r="I22" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="15">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <v>0</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="18" t="s">
+      <c r="C25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>2</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="L23" s="4">
-        <v>1</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="10">
-        <v>1</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="I26" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L26" s="9">
+        <v>1</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="L27" s="9">
+        <v>1</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="9">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
         <v>2</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="L24" s="4">
-        <v>1</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="10">
-        <v>1</v>
-      </c>
-      <c r="F25" s="10">
-        <v>0</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="L25" s="10">
-        <v>1</v>
-      </c>
-      <c r="M25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="10">
-        <v>1</v>
-      </c>
-      <c r="F26" s="10">
-        <v>0</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="L26" s="10">
-        <v>1</v>
-      </c>
-      <c r="M26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="10">
-        <v>1</v>
-      </c>
-      <c r="F27" s="10">
-        <v>0</v>
-      </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="10">
-        <v>1</v>
-      </c>
-      <c r="F28" s="10">
-        <v>0</v>
-      </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1</v>
-      </c>
-      <c r="F29" s="10">
-        <v>0</v>
-      </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11" t="s">
+      <c r="H31" s="17"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K31" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1">
-        <v>2</v>
-      </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="K30" s="11" t="s">
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="1" t="s">
+      <c r="K32" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31" s="18"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11" t="s">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="17"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K33" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="1" t="s">
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11" t="s">
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K34" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33" s="18"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11" t="s">
+      <c r="H35" s="17"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H37" s="17"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K37" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H36" s="18"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11" t="s">
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H38" s="17"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="K38" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H37" s="18"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11" t="s">
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H39" s="17"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="K39" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H38" s="18"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11" t="s">
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H40" s="17"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="K40" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H39" s="18"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="K39" s="11" t="s">
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H41" s="17"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H40" s="18"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11" t="s">
+      <c r="K41" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H42" s="17"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="K40" s="11" t="s">
+      <c r="K42" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H41" s="18"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11" t="s">
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H43" s="17"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="K43" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H42" s="18"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K42" s="11" t="s">
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H44" s="17"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H43" s="18"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11" t="s">
+      <c r="K44" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H45" s="17"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H44" s="18"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11" t="s">
+      <c r="K45" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="K44" s="11" t="s">
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H46" s="17"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H45" s="18"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11" t="s">
+      <c r="K46" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H47" s="17"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="K47" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H46" s="18"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11" t="s">
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H48" s="17"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="K48" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="K46" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H47" s="18"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11" t="s">
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+    </row>
+    <row r="49" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H49" s="17"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="K49" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H48" s="18"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11" t="s">
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H50" s="17"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="K48" s="11" t="s">
+      <c r="K50" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-    </row>
-    <row r="49" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H49" s="18"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11" t="s">
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H51" s="17"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="K49" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-    </row>
-    <row r="50" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H50" s="18"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11" t="s">
+      <c r="K51" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H52" s="17"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="K50" s="11" t="s">
+      <c r="K52" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-    </row>
-    <row r="51" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H51" s="18"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11" t="s">
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+    </row>
+    <row r="53" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H53" s="17"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="K51" s="11" t="s">
+      <c r="K53" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-    </row>
-    <row r="52" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H52" s="18"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="K52" s="11" t="s">
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+    </row>
+    <row r="54" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H54" s="17"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-    </row>
-    <row r="53" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H53" s="18"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11" t="s">
+      <c r="K54" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+    </row>
+    <row r="55" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H55" s="17"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="K53" s="11" t="s">
+      <c r="K55" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-    </row>
-    <row r="54" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H54" s="18"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11" t="s">
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+    </row>
+    <row r="56" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H56" s="17"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="K54" s="11" t="s">
+      <c r="K56" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-    </row>
-    <row r="55" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H55" s="18"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11" t="s">
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+    </row>
+    <row r="57" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H57" s="17"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="K55" s="11" t="s">
+      <c r="K57" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-    </row>
-    <row r="56" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H56" s="18"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="K56" s="11" t="s">
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+    </row>
+    <row r="58" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H58" s="17"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-    </row>
-    <row r="57" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H57" s="18"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11" t="s">
+      <c r="K58" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+    </row>
+    <row r="59" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H59" s="17"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="K57" s="11" t="s">
+      <c r="K59" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-    </row>
-    <row r="58" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H58" s="18"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11" t="s">
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+    </row>
+    <row r="60" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H60" s="17"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="K58" s="11" t="s">
+      <c r="K60" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-    </row>
-    <row r="59" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H59" s="18"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="K59" s="11" t="s">
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+    </row>
+    <row r="61" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H61" s="17"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="K61" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-    </row>
-    <row r="60" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H60" s="18"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11" t="s">
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+    </row>
+    <row r="62" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H62" s="17"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="K60" s="11" t="s">
+      <c r="K62" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-    </row>
-    <row r="61" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H61" s="18"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11" t="s">
+      <c r="L62" s="10"/>
+      <c r="M62" s="10"/>
+    </row>
+    <row r="63" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H63" s="17"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="K63" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="K61" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
-    </row>
-    <row r="62" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H62" s="18"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11" t="s">
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+    </row>
+    <row r="64" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H64" s="17"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="K62" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
-    </row>
-    <row r="63" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H63" s="18"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11" t="s">
+      <c r="K64" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="K63" s="11" t="s">
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
+    </row>
+    <row r="65" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H65" s="17"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="K65" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11"/>
-    </row>
-    <row r="64" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H64" s="18"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11" t="s">
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+    </row>
+    <row r="66" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H66" s="17"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="K64" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-    </row>
-    <row r="65" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H65" s="18"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11" t="s">
+      <c r="K66" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="K65" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="H27:H65"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B8:B17"/>
-    <mergeCell ref="A8:A17"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="G8:G17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="H16:H17"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="G18:G23"/>
     <mergeCell ref="I2:I3"/>
@@ -2855,6 +2856,28 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="N8:N10"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H28:H66"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B8:B17"/>
+    <mergeCell ref="A8:A17"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G8:G17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="H26:H27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>